<commit_message>
Ash Steel Tools & recipes
</commit_message>
<xml_diff>
--- a/D&A.xlsx
+++ b/D&A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\Documents\EX\ForgeDev\Dust_And_Ash_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4124BC4-8C65-455E-8382-B4DF7747E7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2ABB45-8E84-441E-8C82-1B1433F4CC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31812" yWindow="-5280" windowWidth="28800" windowHeight="15432" xr2:uid="{F0DE19EB-6B0E-4876-A78F-5A7BE79C5EE6}"/>
+    <workbookView xWindow="31332" yWindow="-4800" windowWidth="28800" windowHeight="15432" xr2:uid="{F0DE19EB-6B0E-4876-A78F-5A7BE79C5EE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>金</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,32 @@
   </si>
   <si>
     <t>金，金属</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ff0000</t>
+  </si>
+  <si>
+    <t>00ff44</t>
+  </si>
+  <si>
+    <t>energy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00aaff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜色加深</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50%+50%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -292,7 +318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -300,6 +326,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,7 +650,7 @@
   <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -717,6 +746,18 @@
       <c r="C13" t="s">
         <v>40</v>
       </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>128</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
@@ -725,6 +766,9 @@
       <c r="C14" t="s">
         <v>41</v>
       </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -733,6 +777,9 @@
       <c r="C15" t="s">
         <v>42</v>
       </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -741,88 +788,135 @@
       <c r="C16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>884400</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>777777</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>18</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>21</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>22</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>23</v>
       </c>

</xml_diff>